<commit_message>
reworking 2 script, none of them finish yet
</commit_message>
<xml_diff>
--- a/Greenbox/กล่องเขียว.xlsx
+++ b/Greenbox/กล่องเขียว.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Greenbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF291220-F5F3-4E1E-ABD2-55E7193A1A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84DD3EB-3A31-4C2F-88EF-9723FD554134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="675" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="เขียว" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+  <si>
+    <t>SVCOM7-654/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-246/0018</t>
+  </si>
+  <si>
+    <t>SVCOM7-844/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-695/0014</t>
+  </si>
+  <si>
+    <t>SVCOM7-486/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-667/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-469/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-413/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-683/0018</t>
+  </si>
+  <si>
+    <t>SVCOM7-472/0016</t>
+  </si>
+  <si>
+    <t>SVCOM7-732/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-1085/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-1113/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-215/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-233/0014</t>
+  </si>
+  <si>
+    <t>SVCOM7-914/0012</t>
+  </si>
+  <si>
+    <t>SVCOM7-683/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-543/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-498/0016</t>
+  </si>
+  <si>
+    <t>SVCOM7-693/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-498/0008</t>
+  </si>
+  <si>
+    <t>29/8/2022</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -55,12 +128,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,14 +435,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1">
+        <v>171</v>
+      </c>
+      <c r="C1" s="1">
+        <v>654</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1">
+        <v>379</v>
+      </c>
+      <c r="C2" s="1">
+        <v>246</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1">
+        <v>169</v>
+      </c>
+      <c r="C3" s="1">
+        <v>844</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
+        <v>200</v>
+      </c>
+      <c r="C4" s="1">
+        <v>695</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>86</v>
+      </c>
+      <c r="C5" s="1">
+        <v>486</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>147</v>
+      </c>
+      <c r="C6" s="1">
+        <v>667</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1">
+        <v>120</v>
+      </c>
+      <c r="C7" s="1">
+        <v>469</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1">
+        <v>242</v>
+      </c>
+      <c r="C8" s="1">
+        <v>413</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1">
+        <v>939</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>340</v>
+      </c>
+      <c r="C10" s="1">
+        <v>683</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1">
+        <v>234</v>
+      </c>
+      <c r="C11" s="1">
+        <v>472</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>85</v>
+      </c>
+      <c r="C12" s="1">
+        <v>732</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1">
+        <v>99</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1085</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>256</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1113</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1">
+        <v>198</v>
+      </c>
+      <c r="C15" s="1">
+        <v>215</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>581</v>
+      </c>
+      <c r="C16" s="1">
+        <v>233</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
+        <v>198</v>
+      </c>
+      <c r="C17" s="1">
+        <v>914</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1">
+        <v>339</v>
+      </c>
+      <c r="C18" s="1">
+        <v>683</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>154</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1086</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1">
+        <v>375</v>
+      </c>
+      <c r="C20" s="1">
+        <v>498</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1">
+        <v>150</v>
+      </c>
+      <c r="C21" s="1">
+        <v>693</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>374</v>
+      </c>
+      <c r="C22" s="1">
+        <v>498</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
prepare for sidesticker script
</commit_message>
<xml_diff>
--- a/Greenbox/กล่องเขียว.xlsx
+++ b/Greenbox/กล่องเขียว.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Greenbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84DD3EB-3A31-4C2F-88EF-9723FD554134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EAA60A-4F27-409C-8352-1DA8DA95BF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="675" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="915" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="เขียว" sheetId="1" r:id="rId1"/>
@@ -25,72 +25,294 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
-  <si>
-    <t>SVCOM7-654/0009</t>
-  </si>
-  <si>
-    <t>SVCOM7-246/0018</t>
-  </si>
-  <si>
-    <t>SVCOM7-844/0001</t>
-  </si>
-  <si>
-    <t>SVCOM7-695/0014</t>
-  </si>
-  <si>
-    <t>SVCOM7-486/0009</t>
-  </si>
-  <si>
-    <t>SVCOM7-667/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-469/0002</t>
-  </si>
-  <si>
-    <t>SVCOM7-413/0009</t>
-  </si>
-  <si>
-    <t>SVCOM7-683/0018</t>
-  </si>
-  <si>
-    <t>SVCOM7-472/0016</t>
-  </si>
-  <si>
-    <t>SVCOM7-732/0006</t>
-  </si>
-  <si>
-    <t>SVCOM7-1085/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-1113/0008</t>
-  </si>
-  <si>
-    <t>SVCOM7-215/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-233/0014</t>
-  </si>
-  <si>
-    <t>SVCOM7-914/0012</t>
-  </si>
-  <si>
-    <t>SVCOM7-683/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-543/0006</t>
-  </si>
-  <si>
-    <t>SVCOM7-498/0016</t>
-  </si>
-  <si>
-    <t>SVCOM7-693/0001</t>
-  </si>
-  <si>
-    <t>SVCOM7-498/0008</t>
-  </si>
-  <si>
-    <t>29/8/2022</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
+  <si>
+    <t>SVCOM7-249/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-53/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-754/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-660/0016</t>
+  </si>
+  <si>
+    <t>SVCOM7-740/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-748/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-163/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-1403/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-754/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-138/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-1403/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-748/0018</t>
+  </si>
+  <si>
+    <t>SVCOM7-700/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-321/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-410/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-168/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-776/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-776/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-286/0013</t>
+  </si>
+  <si>
+    <t>SVCOM7-1069/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-676/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-543/0018</t>
+  </si>
+  <si>
+    <t>SVCOM7-633/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-363/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-413/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-389/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-543/0015</t>
+  </si>
+  <si>
+    <t>SVCOM7-246/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-486/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-653/0020</t>
+  </si>
+  <si>
+    <t>SVCOM7-282/0016</t>
+  </si>
+  <si>
+    <t>SVCOM7-1376/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-282/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-625/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-1317/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-1616/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-216/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-844/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-340/0013</t>
+  </si>
+  <si>
+    <t>SVCOM7-356/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-414/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-465/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-465/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-633/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-775/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-398/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-263/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-633/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-584/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-1399/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-138/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-661/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-740/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-105/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-869/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-410/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-206/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-321/0020</t>
+  </si>
+  <si>
+    <t>SVCOM7-292/0015</t>
+  </si>
+  <si>
+    <t>SVCOM7-725/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-233/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-865/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-869/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-654/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-691/0019</t>
+  </si>
+  <si>
+    <t>SVCOM7-1195/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-216/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-498/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-104/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-392/0015</t>
+  </si>
+  <si>
+    <t>SVCOM7-1196/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-499/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-776/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-282/0015</t>
+  </si>
+  <si>
+    <t>SVCOM7-695/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-1560/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-370/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-939/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-292/0012</t>
+  </si>
+  <si>
+    <t>SVCOM7-245/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-797/0017</t>
+  </si>
+  <si>
+    <t>SVCOM7-329/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-784/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-651/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-31/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-914/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-914/0011</t>
+  </si>
+  <si>
+    <t>SVCOM7-674/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-414/0014</t>
+  </si>
+  <si>
+    <t>SVCOM7-741/0018</t>
+  </si>
+  <si>
+    <t>SVCOM7-472/0011</t>
+  </si>
+  <si>
+    <t>SVCOM7-683/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-387/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-233/0009</t>
+  </si>
+  <si>
+    <t>30/8/2022</t>
+  </si>
+  <si>
+    <t>31/8/2022</t>
   </si>
 </sst>
 </file>
@@ -435,23 +657,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1">
-        <v>171</v>
+        <v>262</v>
       </c>
       <c r="C1" s="1">
-        <v>654</v>
+        <v>249</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -459,13 +681,13 @@
     </row>
     <row r="2" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1">
-        <v>379</v>
+        <v>335</v>
       </c>
       <c r="C2" s="1">
-        <v>246</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -473,13 +695,13 @@
     </row>
     <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1">
-        <v>169</v>
+        <v>395</v>
       </c>
       <c r="C3" s="1">
-        <v>844</v>
+        <v>754</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -487,13 +709,13 @@
     </row>
     <row r="4" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="C4" s="1">
-        <v>695</v>
+        <v>660</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -501,13 +723,13 @@
     </row>
     <row r="5" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1">
         <v>86</v>
       </c>
       <c r="C5" s="1">
-        <v>486</v>
+        <v>740</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -515,13 +737,13 @@
     </row>
     <row r="6" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1">
-        <v>147</v>
+        <v>610</v>
       </c>
       <c r="C6" s="1">
-        <v>667</v>
+        <v>748</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -529,27 +751,27 @@
     </row>
     <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B7" s="1">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1">
-        <v>469</v>
+        <v>163</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1">
-        <v>242</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>413</v>
+        <v>1403</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -557,13 +779,13 @@
     </row>
     <row r="9" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B9" s="1">
-        <v>65</v>
+        <v>396</v>
       </c>
       <c r="C9" s="1">
-        <v>939</v>
+        <v>754</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -571,184 +793,1192 @@
     </row>
     <row r="10" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1">
-        <v>340</v>
+        <v>892</v>
       </c>
       <c r="C10" s="1">
-        <v>683</v>
+        <v>138</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1">
-        <v>234</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1">
-        <v>472</v>
+        <v>1403</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1">
-        <v>85</v>
+        <v>609</v>
       </c>
       <c r="C12" s="1">
-        <v>732</v>
+        <v>748</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1">
-        <v>1085</v>
+        <v>700</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1">
-        <v>256</v>
+        <v>367</v>
       </c>
       <c r="C14" s="1">
-        <v>1113</v>
+        <v>321</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1">
-        <v>198</v>
+        <v>511</v>
       </c>
       <c r="C15" s="1">
-        <v>215</v>
+        <v>410</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1">
-        <v>581</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1">
-        <v>233</v>
+        <v>168</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C17" s="1">
-        <v>914</v>
+        <v>776</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1">
-        <v>339</v>
+        <v>189</v>
       </c>
       <c r="C18" s="1">
-        <v>683</v>
+        <v>776</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B19" s="1">
-        <v>154</v>
+        <v>221</v>
       </c>
       <c r="C19" s="1">
-        <v>1086</v>
+        <v>286</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B20" s="1">
-        <v>375</v>
+        <v>184</v>
       </c>
       <c r="C20" s="1">
-        <v>498</v>
+        <v>1069</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B21" s="1">
-        <v>150</v>
+        <v>319</v>
       </c>
       <c r="C21" s="1">
-        <v>693</v>
+        <v>676</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="1">
+        <v>300</v>
+      </c>
+      <c r="C22" s="1">
+        <v>543</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
-        <v>374</v>
-      </c>
-      <c r="C22" s="1">
+    </row>
+    <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1223</v>
+      </c>
+      <c r="C23" s="1">
+        <v>633</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="1">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1">
+        <v>363</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1">
+        <v>243</v>
+      </c>
+      <c r="C25" s="1">
+        <v>413</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="1">
+        <v>72</v>
+      </c>
+      <c r="C26" s="1">
+        <v>389</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="1">
+        <v>301</v>
+      </c>
+      <c r="C27" s="1">
+        <v>543</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="1">
+        <v>381</v>
+      </c>
+      <c r="C28" s="1">
+        <v>246</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="1">
+        <v>89</v>
+      </c>
+      <c r="C29" s="1">
+        <v>486</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="1">
+        <v>476</v>
+      </c>
+      <c r="C30" s="1">
+        <v>653</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="1">
+        <v>211</v>
+      </c>
+      <c r="C31" s="1">
+        <v>282</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="1">
+        <v>98</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1376</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="1">
+        <v>211</v>
+      </c>
+      <c r="C33" s="1">
+        <v>282</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="1">
+        <v>62</v>
+      </c>
+      <c r="C34" s="1">
+        <v>625</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1">
+        <v>32</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1317</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1616</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="1">
+        <v>426</v>
+      </c>
+      <c r="C37" s="1">
+        <v>216</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="1">
+        <v>170</v>
+      </c>
+      <c r="C38" s="1">
+        <v>844</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="1">
+        <v>501</v>
+      </c>
+      <c r="C39" s="1">
+        <v>337</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="1">
+        <v>115</v>
+      </c>
+      <c r="C40" s="1">
+        <v>356</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="1">
+        <v>252</v>
+      </c>
+      <c r="C41" s="1">
+        <v>414</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="1">
+        <v>99</v>
+      </c>
+      <c r="C42" s="1">
+        <v>465</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="1">
+        <v>98</v>
+      </c>
+      <c r="C43" s="1">
+        <v>465</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1226</v>
+      </c>
+      <c r="C44" s="1">
+        <v>633</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="1">
+        <v>210</v>
+      </c>
+      <c r="C45" s="1">
+        <v>775</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="1">
+        <v>160</v>
+      </c>
+      <c r="C46" s="1">
+        <v>398</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="1">
+        <v>81</v>
+      </c>
+      <c r="C47" s="1">
+        <v>263</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1227</v>
+      </c>
+      <c r="C48" s="1">
+        <v>633</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="1">
+        <v>81</v>
+      </c>
+      <c r="C49" s="1">
+        <v>584</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="1">
+        <v>72</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1399</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="1">
+        <v>894</v>
+      </c>
+      <c r="C51" s="1">
+        <v>138</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="1">
+        <v>244</v>
+      </c>
+      <c r="C52" s="1">
+        <v>661</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" s="1">
+        <v>87</v>
+      </c>
+      <c r="C53" s="1">
+        <v>740</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="1">
+        <v>449</v>
+      </c>
+      <c r="C54" s="1">
+        <v>105</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="1">
+        <v>144</v>
+      </c>
+      <c r="C55" s="1">
+        <v>869</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" s="1">
+        <v>512</v>
+      </c>
+      <c r="C56" s="1">
+        <v>410</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" s="1">
+        <v>219</v>
+      </c>
+      <c r="C57" s="1">
+        <v>206</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="1">
+        <v>368</v>
+      </c>
+      <c r="C58" s="1">
+        <v>321</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="1">
+        <v>665</v>
+      </c>
+      <c r="C59" s="1">
+        <v>292</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="1">
+        <v>134</v>
+      </c>
+      <c r="C60" s="1">
+        <v>725</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="1">
+        <v>584</v>
+      </c>
+      <c r="C61" s="1">
+        <v>233</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="1">
+        <v>112</v>
+      </c>
+      <c r="C62" s="1">
+        <v>865</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="1">
+        <v>143</v>
+      </c>
+      <c r="C63" s="1">
+        <v>869</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64" s="1">
+        <v>173</v>
+      </c>
+      <c r="C64" s="1">
+        <v>654</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" s="1">
+        <v>525</v>
+      </c>
+      <c r="C65" s="1">
+        <v>691</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="1">
+        <v>35</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1195</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" s="1">
+        <v>427</v>
+      </c>
+      <c r="C67" s="1">
+        <v>216</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="1">
+        <v>377</v>
+      </c>
+      <c r="C68" s="1">
         <v>498</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>20</v>
+      <c r="D68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69" s="1">
+        <v>219</v>
+      </c>
+      <c r="C69" s="1">
+        <v>104</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="1">
+        <v>241</v>
+      </c>
+      <c r="C70" s="1">
+        <v>392</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" s="1">
+        <v>108</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1196</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="1">
+        <v>132</v>
+      </c>
+      <c r="C72" s="1">
+        <v>499</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73" s="1">
+        <v>190</v>
+      </c>
+      <c r="C73" s="1">
+        <v>776</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" s="1">
+        <v>212</v>
+      </c>
+      <c r="C74" s="1">
+        <v>282</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="1">
+        <v>201</v>
+      </c>
+      <c r="C75" s="1">
+        <v>695</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76" s="1">
+        <v>81</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1560</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" s="1">
+        <v>173</v>
+      </c>
+      <c r="C77" s="1">
+        <v>370</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" s="1">
+        <v>66</v>
+      </c>
+      <c r="C78" s="1">
+        <v>939</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" s="1">
+        <v>664</v>
+      </c>
+      <c r="C79" s="1">
+        <v>292</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" s="1">
+        <v>108</v>
+      </c>
+      <c r="C80" s="1">
+        <v>245</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B81" s="1">
+        <v>214</v>
+      </c>
+      <c r="C81" s="1">
+        <v>797</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B82" s="1">
+        <v>630</v>
+      </c>
+      <c r="C82" s="1">
+        <v>329</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" s="1">
+        <v>91</v>
+      </c>
+      <c r="C83" s="1">
+        <v>784</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" s="1">
+        <v>240</v>
+      </c>
+      <c r="C84" s="1">
+        <v>651</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85" s="1">
+        <v>80</v>
+      </c>
+      <c r="C85" s="1">
+        <v>31</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86" s="1">
+        <v>200</v>
+      </c>
+      <c r="C86" s="1">
+        <v>914</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="1">
+        <v>199</v>
+      </c>
+      <c r="C87" s="1">
+        <v>914</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" s="1">
+        <v>328</v>
+      </c>
+      <c r="C88" s="1">
+        <v>674</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B89" s="1">
+        <v>253</v>
+      </c>
+      <c r="C89" s="1">
+        <v>414</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90" s="1">
+        <v>277</v>
+      </c>
+      <c r="C90" s="1">
+        <v>741</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="1">
+        <v>235</v>
+      </c>
+      <c r="C91" s="1">
+        <v>472</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" s="1">
+        <v>341</v>
+      </c>
+      <c r="C92" s="1">
+        <v>683</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" s="1">
+        <v>99</v>
+      </c>
+      <c r="C93" s="1">
+        <v>387</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" s="1">
+        <v>583</v>
+      </c>
+      <c r="C94" s="1">
+        <v>233</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented error catch for stock in
</commit_message>
<xml_diff>
--- a/Greenbox/กล่องเขียว.xlsx
+++ b/Greenbox/กล่องเขียว.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Greenbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08EB506-8368-45A2-BC7E-6DF8B7C05421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1190BC00-1C36-41E2-8E50-E833D833331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="1620" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="เขียว" sheetId="1" r:id="rId1"/>
@@ -33,135 +33,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
-  <si>
-    <t>SVCOM7-740/0009</t>
-  </si>
-  <si>
-    <t>SVCOM7-750/1:304</t>
-  </si>
-  <si>
-    <t>SVCOM7-914/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-749/0015</t>
-  </si>
-  <si>
-    <t>SVCOM7-175/0009</t>
-  </si>
-  <si>
-    <t>SVCOM7-469/0008</t>
-  </si>
-  <si>
-    <t>SVCOM7-740/0008</t>
-  </si>
-  <si>
-    <t>SVCOM7-749/0013</t>
-  </si>
-  <si>
-    <t>SVCOM7-175/0016</t>
-  </si>
-  <si>
-    <t>SVCOM7-1069/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-1399/0006</t>
-  </si>
-  <si>
-    <t>SVCOM7-233/0018</t>
-  </si>
-  <si>
-    <t>SVCOM7-249/0019</t>
-  </si>
-  <si>
-    <t>SVCOM7-286/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-683/0002</t>
-  </si>
-  <si>
-    <t>SVCOM7-498/0012</t>
-  </si>
-  <si>
-    <t>SVCOM7-653/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-443/0001</t>
-  </si>
-  <si>
-    <t>SVCOM7-740/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-754/0010</t>
-  </si>
-  <si>
-    <t>SVCOM7-486/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-661/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-206/0002</t>
-  </si>
-  <si>
-    <t>SVCOM7-719/0010</t>
-  </si>
-  <si>
-    <t>SVCOM7-413/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-675/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-1616/0009</t>
-  </si>
-  <si>
-    <t>SVCOM7-206/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-784/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-388/0001</t>
-  </si>
-  <si>
-    <t>SVCOM7-720/0008</t>
-  </si>
-  <si>
-    <t>SVCOM7-1376/0005</t>
-  </si>
-  <si>
-    <t>SVCOM7-282/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-263/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-104/0020</t>
-  </si>
-  <si>
-    <t>SVCOM7-356/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-748/0001</t>
-  </si>
-  <si>
-    <t>SVCOM7-192/0009</t>
-  </si>
-  <si>
-    <t>SVCOM7-720/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-1382/0010</t>
-  </si>
-  <si>
-    <t>SVCOM7-175/0015</t>
-  </si>
-  <si>
-    <t>SVCOM7-371/0006</t>
-  </si>
-  <si>
-    <t>7/9/2022</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+  <si>
+    <t>SVCOM7-206/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-105/0020</t>
+  </si>
+  <si>
+    <t>SVCOM7-1317/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-676/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-263/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-286/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-138/0020</t>
+  </si>
+  <si>
+    <t>SVCOM7-465/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-647/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-396/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-748/0017</t>
+  </si>
+  <si>
+    <t>SVCOM7-1075/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-1382/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-797/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-363/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-639/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-245/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-321/0016</t>
+  </si>
+  <si>
+    <t>SVCOM7-748/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-341/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-337/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-1616/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-292/0019</t>
+  </si>
+  <si>
+    <t>SVCOM7-844/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-1405/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-673/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-410/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-53/0016</t>
+  </si>
+  <si>
+    <t>SVCOM7-286/0019</t>
+  </si>
+  <si>
+    <t>SVCOM7-633/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-869/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-1069/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-499/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-105/0017</t>
+  </si>
+  <si>
+    <t>SVCOM7-653/0017</t>
+  </si>
+  <si>
+    <t>SVCOM7-654/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-329/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-472/0003</t>
+  </si>
+  <si>
+    <t>10/9/2022</t>
+  </si>
+  <si>
+    <t>11/9/2022</t>
+  </si>
+  <si>
+    <t>12/9/2022</t>
   </si>
 </sst>
 </file>
@@ -506,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -516,41 +510,41 @@
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1">
-        <v>88</v>
+        <v>223</v>
       </c>
       <c r="C1" s="1">
-        <v>740</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1">
-        <v>49</v>
+        <v>456</v>
       </c>
       <c r="C2" s="1">
-        <v>750</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1">
-        <v>204</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1">
-        <v>914</v>
+        <v>1317</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -558,13 +552,13 @@
     </row>
     <row r="4" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1">
-        <v>243</v>
+        <v>325</v>
       </c>
       <c r="C4" s="1">
-        <v>749</v>
+        <v>676</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -572,13 +566,13 @@
     </row>
     <row r="5" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1">
-        <v>639</v>
+        <v>263</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -586,13 +580,13 @@
     </row>
     <row r="6" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="C6" s="1">
-        <v>469</v>
+        <v>286</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -600,13 +594,13 @@
     </row>
     <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1">
-        <v>89</v>
+        <v>898</v>
       </c>
       <c r="C7" s="1">
-        <v>740</v>
+        <v>138</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -614,13 +608,13 @@
     </row>
     <row r="8" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1">
-        <v>244</v>
+        <v>100</v>
       </c>
       <c r="C8" s="1">
-        <v>749</v>
+        <v>465</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -628,69 +622,69 @@
     </row>
     <row r="9" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1">
-        <v>115</v>
+        <v>556</v>
       </c>
       <c r="C9" s="1">
-        <v>639</v>
+        <v>647</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
-        <v>188</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1">
-        <v>1069</v>
+        <v>975</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1">
-        <v>73</v>
+        <v>619</v>
       </c>
       <c r="C11" s="1">
-        <v>1399</v>
+        <v>748</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1">
-        <v>587</v>
+        <v>97</v>
       </c>
       <c r="C12" s="1">
-        <v>233</v>
+        <v>1075</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1">
-        <v>270</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1">
-        <v>249</v>
+        <v>1382</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -698,13 +692,13 @@
     </row>
     <row r="14" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C14" s="1">
-        <v>286</v>
+        <v>797</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -712,13 +706,13 @@
     </row>
     <row r="15" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
-        <v>344</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1">
-        <v>683</v>
+        <v>363</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>14</v>
@@ -726,13 +720,13 @@
     </row>
     <row r="16" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1">
-        <v>380</v>
+        <v>118</v>
       </c>
       <c r="C16" s="1">
-        <v>498</v>
+        <v>639</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>15</v>
@@ -740,13 +734,13 @@
     </row>
     <row r="17" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1">
-        <v>478</v>
+        <v>110</v>
       </c>
       <c r="C17" s="1">
-        <v>653</v>
+        <v>245</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
@@ -754,13 +748,13 @@
     </row>
     <row r="18" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1">
-        <v>147</v>
+        <v>376</v>
       </c>
       <c r="C18" s="1">
-        <v>443</v>
+        <v>321</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -768,13 +762,13 @@
     </row>
     <row r="19" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1">
-        <v>90</v>
+        <v>617</v>
       </c>
       <c r="C19" s="1">
-        <v>740</v>
+        <v>748</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>18</v>
@@ -782,13 +776,13 @@
     </row>
     <row r="20" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="1">
-        <v>404</v>
+        <v>123</v>
       </c>
       <c r="C20" s="1">
-        <v>754</v>
+        <v>341</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -796,27 +790,27 @@
     </row>
     <row r="21" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1">
-        <v>98</v>
+        <v>506</v>
       </c>
       <c r="C21" s="1">
-        <v>486</v>
+        <v>337</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1">
-        <v>248</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1">
-        <v>661</v>
+        <v>1616</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>21</v>
@@ -824,13 +818,13 @@
     </row>
     <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1">
-        <v>222</v>
+        <v>672</v>
       </c>
       <c r="C23" s="1">
-        <v>206</v>
+        <v>292</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>22</v>
@@ -838,27 +832,27 @@
     </row>
     <row r="24" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1">
-        <v>719</v>
+        <v>844</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1">
-        <v>251</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1">
-        <v>413</v>
+        <v>1405</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>24</v>
@@ -866,27 +860,27 @@
     </row>
     <row r="26" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1">
-        <v>446</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1">
-        <v>46</v>
+        <v>524</v>
       </c>
       <c r="C27" s="1">
-        <v>1616</v>
+        <v>410</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>26</v>
@@ -894,13 +888,13 @@
     </row>
     <row r="28" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1">
-        <v>220</v>
+        <v>341</v>
       </c>
       <c r="C28" s="1">
-        <v>206</v>
+        <v>53</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
@@ -908,13 +902,13 @@
     </row>
     <row r="29" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B29" s="1">
-        <v>93</v>
+        <v>226</v>
       </c>
       <c r="C29" s="1">
-        <v>784</v>
+        <v>286</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>28</v>
@@ -922,13 +916,13 @@
     </row>
     <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1">
-        <v>8</v>
+        <v>1235</v>
       </c>
       <c r="C30" s="1">
-        <v>388</v>
+        <v>633</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>29</v>
@@ -936,13 +930,13 @@
     </row>
     <row r="31" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="C31" s="1">
-        <v>720</v>
+        <v>869</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>30</v>
@@ -950,13 +944,13 @@
     </row>
     <row r="32" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1">
-        <v>106</v>
+        <v>189</v>
       </c>
       <c r="C32" s="1">
-        <v>1376</v>
+        <v>1069</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>31</v>
@@ -964,13 +958,13 @@
     </row>
     <row r="33" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1">
-        <v>214</v>
+        <v>136</v>
       </c>
       <c r="C33" s="1">
-        <v>282</v>
+        <v>499</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>32</v>
@@ -978,13 +972,13 @@
     </row>
     <row r="34" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1">
-        <v>83</v>
+        <v>458</v>
       </c>
       <c r="C34" s="1">
-        <v>263</v>
+        <v>105</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>33</v>
@@ -992,13 +986,13 @@
     </row>
     <row r="35" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1">
-        <v>222</v>
+        <v>481</v>
       </c>
       <c r="C35" s="1">
-        <v>104</v>
+        <v>653</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>34</v>
@@ -1006,13 +1000,13 @@
     </row>
     <row r="36" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="C36" s="1">
-        <v>356</v>
+        <v>654</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>35</v>
@@ -1020,13 +1014,13 @@
     </row>
     <row r="37" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1">
-        <v>615</v>
+        <v>641</v>
       </c>
       <c r="C37" s="1">
-        <v>748</v>
+        <v>329</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>36</v>
@@ -1034,72 +1028,16 @@
     </row>
     <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C38" s="1">
-        <v>192</v>
+        <v>472</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="1">
-        <v>78</v>
-      </c>
-      <c r="C39" s="1">
-        <v>720</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="1">
-        <v>20</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1382</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="1">
-        <v>114</v>
-      </c>
-      <c r="C41" s="1">
-        <v>639</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="1">
-        <v>152</v>
-      </c>
-      <c r="C42" s="1">
-        <v>371</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added foundstockbill pic asset
</commit_message>
<xml_diff>
--- a/Greenbox/กล่องเขียว.xlsx
+++ b/Greenbox/กล่องเขียว.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workstuff\my-work-python-script\Greenbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1190BC00-1C36-41E2-8E50-E833D833331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E22E61-FD47-40AF-A93E-0C9C61B26910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="1620" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="เขียว" sheetId="1" r:id="rId1"/>
@@ -33,129 +33,174 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
-  <si>
-    <t>SVCOM7-206/0006</t>
-  </si>
-  <si>
-    <t>SVCOM7-105/0020</t>
-  </si>
-  <si>
-    <t>SVCOM7-1317/0005</t>
-  </si>
-  <si>
-    <t>SVCOM7-676/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-263/0001</t>
-  </si>
-  <si>
-    <t>SVCOM7-286/0005</t>
-  </si>
-  <si>
-    <t>SVCOM7-138/0020</t>
-  </si>
-  <si>
-    <t>SVCOM7-465/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-647/0005</t>
-  </si>
-  <si>
-    <t>SVCOM7-396/0006</t>
-  </si>
-  <si>
-    <t>SVCOM7-748/0017</t>
-  </si>
-  <si>
-    <t>SVCOM7-1075/0002</t>
-  </si>
-  <si>
-    <t>SVCOM7-1382/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-797/0008</t>
-  </si>
-  <si>
-    <t>SVCOM7-363/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-639/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-245/0008</t>
-  </si>
-  <si>
-    <t>SVCOM7-321/0016</t>
-  </si>
-  <si>
-    <t>SVCOM7-748/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-341/0006</t>
-  </si>
-  <si>
-    <t>SVCOM7-337/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-1616/0005</t>
-  </si>
-  <si>
-    <t>SVCOM7-292/0019</t>
-  </si>
-  <si>
-    <t>SVCOM7-844/0005</t>
-  </si>
-  <si>
-    <t>SVCOM7-1405/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-673/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-410/0008</t>
-  </si>
-  <si>
-    <t>SVCOM7-53/0016</t>
-  </si>
-  <si>
-    <t>SVCOM7-286/0019</t>
-  </si>
-  <si>
-    <t>SVCOM7-633/0004</t>
-  </si>
-  <si>
-    <t>SVCOM7-869/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-1069/0002</t>
-  </si>
-  <si>
-    <t>SVCOM7-499/0005</t>
-  </si>
-  <si>
-    <t>SVCOM7-105/0017</t>
-  </si>
-  <si>
-    <t>SVCOM7-653/0017</t>
-  </si>
-  <si>
-    <t>SVCOM7-654/0007</t>
-  </si>
-  <si>
-    <t>SVCOM7-329/0003</t>
-  </si>
-  <si>
-    <t>SVCOM7-472/0003</t>
-  </si>
-  <si>
-    <t>10/9/2022</t>
-  </si>
-  <si>
-    <t>11/9/2022</t>
-  </si>
-  <si>
-    <t>12/9/2022</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+  <si>
+    <t>SVCOM7-115/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-215/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-720/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-1376/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-1554/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-654/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-632/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-653/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-168/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-305/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-340/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-1113/0016</t>
+  </si>
+  <si>
+    <t>SVCOM7-53/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-691-0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-749/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-973/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-660/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-2075/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-939/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-1405/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-667/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-321/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-298/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-1086/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-691/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-1113/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-741/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-633/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-973/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-387/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-1196/0003</t>
+  </si>
+  <si>
+    <t>SVCOM7-337/0014</t>
+  </si>
+  <si>
+    <t>SVCOM7-398/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-776/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-748/0014</t>
+  </si>
+  <si>
+    <t>SVCOM7-633/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-1196/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-719/0008</t>
+  </si>
+  <si>
+    <t>SVCOM7-370/0004</t>
+  </si>
+  <si>
+    <t>SVCOM7-684/0007</t>
+  </si>
+  <si>
+    <t>SVCOM7-321/0013</t>
+  </si>
+  <si>
+    <t>SVCOM7-844/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-776/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-686/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-396/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-246/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-691/0010</t>
+  </si>
+  <si>
+    <t>SVCOM7-674/0015</t>
+  </si>
+  <si>
+    <t>SVCOM7-334/0002</t>
+  </si>
+  <si>
+    <t>SVCOM7-246/0009</t>
+  </si>
+  <si>
+    <t>SVCOM7-780/0005</t>
+  </si>
+  <si>
+    <t>SVCOM7-207/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-774/0001</t>
+  </si>
+  <si>
+    <t>SVCOM7-104/0006</t>
+  </si>
+  <si>
+    <t>SVCOM7-329/0550</t>
+  </si>
+  <si>
+    <t>13/9/2022</t>
   </si>
 </sst>
 </file>
@@ -500,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -510,13 +555,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1">
-        <v>223</v>
+        <v>376</v>
       </c>
       <c r="C1" s="1">
-        <v>206</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -524,55 +569,55 @@
     </row>
     <row r="2" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1">
-        <v>456</v>
+        <v>208</v>
       </c>
       <c r="C2" s="1">
-        <v>105</v>
+        <v>215</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1">
-        <v>1317</v>
+        <v>720</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1">
-        <v>325</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1">
-        <v>676</v>
+        <v>1376</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1">
-        <v>263</v>
+        <v>1554</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -580,13 +625,13 @@
     </row>
     <row r="6" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="C6" s="1">
-        <v>286</v>
+        <v>654</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -594,13 +639,13 @@
     </row>
     <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1">
-        <v>898</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1">
-        <v>138</v>
+        <v>632</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -608,13 +653,13 @@
     </row>
     <row r="8" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1">
-        <v>100</v>
+        <v>482</v>
       </c>
       <c r="C8" s="1">
-        <v>465</v>
+        <v>653</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -622,13 +667,13 @@
     </row>
     <row r="9" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1">
-        <v>556</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1">
-        <v>647</v>
+        <v>168</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -636,13 +681,13 @@
     </row>
     <row r="10" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1">
-        <v>26</v>
+        <v>234</v>
       </c>
       <c r="C10" s="1">
-        <v>975</v>
+        <v>305</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -650,13 +695,13 @@
     </row>
     <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1">
-        <v>619</v>
+        <v>370</v>
       </c>
       <c r="C11" s="1">
-        <v>748</v>
+        <v>340</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
@@ -664,27 +709,27 @@
     </row>
     <row r="12" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1">
-        <v>97</v>
+        <v>267</v>
       </c>
       <c r="C12" s="1">
-        <v>1075</v>
+        <v>1113</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1">
-        <v>23</v>
+        <v>342</v>
       </c>
       <c r="C13" s="1">
-        <v>1382</v>
+        <v>53</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -692,13 +737,13 @@
     </row>
     <row r="14" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
-        <v>217</v>
+        <v>531</v>
       </c>
       <c r="C14" s="1">
-        <v>797</v>
+        <v>691</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -706,13 +751,13 @@
     </row>
     <row r="15" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1">
-        <v>89</v>
+        <v>248</v>
       </c>
       <c r="C15" s="1">
-        <v>363</v>
+        <v>749</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>14</v>
@@ -720,13 +765,13 @@
     </row>
     <row r="16" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
-        <v>639</v>
+        <v>1752</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>15</v>
@@ -734,27 +779,27 @@
     </row>
     <row r="17" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1">
-        <v>110</v>
+        <v>251</v>
       </c>
       <c r="C17" s="1">
-        <v>245</v>
+        <v>660</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1">
-        <v>376</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1">
-        <v>321</v>
+        <v>2075</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -762,27 +807,27 @@
     </row>
     <row r="19" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1">
-        <v>617</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1">
-        <v>748</v>
+        <v>939</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1">
-        <v>341</v>
+        <v>1405</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -790,27 +835,27 @@
     </row>
     <row r="21" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1">
-        <v>506</v>
+        <v>156</v>
       </c>
       <c r="C21" s="1">
-        <v>337</v>
+        <v>667</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1">
-        <v>48</v>
+        <v>377</v>
       </c>
       <c r="C22" s="1">
-        <v>1616</v>
+        <v>321</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>21</v>
@@ -818,55 +863,55 @@
     </row>
     <row r="23" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1">
-        <v>672</v>
+        <v>349</v>
       </c>
       <c r="C23" s="1">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="C24" s="1">
-        <v>844</v>
+        <v>1086</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1">
-        <v>14</v>
+        <v>532</v>
       </c>
       <c r="C25" s="1">
-        <v>1405</v>
+        <v>691</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1">
-        <v>68</v>
+        <v>268</v>
       </c>
       <c r="C26" s="1">
-        <v>673</v>
+        <v>1113</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>25</v>
@@ -874,13 +919,13 @@
     </row>
     <row r="27" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1">
-        <v>524</v>
+        <v>284</v>
       </c>
       <c r="C27" s="1">
-        <v>410</v>
+        <v>741</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>26</v>
@@ -888,13 +933,13 @@
     </row>
     <row r="28" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B28" s="1">
-        <v>341</v>
+        <v>1237</v>
       </c>
       <c r="C28" s="1">
-        <v>53</v>
+        <v>633</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
@@ -902,13 +947,13 @@
     </row>
     <row r="29" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1">
-        <v>226</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1">
-        <v>286</v>
+        <v>1752</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>28</v>
@@ -916,41 +961,41 @@
     </row>
     <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1">
-        <v>1235</v>
+        <v>100</v>
       </c>
       <c r="C30" s="1">
-        <v>633</v>
+        <v>387</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1">
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="C31" s="1">
-        <v>869</v>
+        <v>1196</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B32" s="1">
-        <v>189</v>
+        <v>509</v>
       </c>
       <c r="C32" s="1">
-        <v>1069</v>
+        <v>337</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>31</v>
@@ -958,13 +1003,13 @@
     </row>
     <row r="33" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="C33" s="1">
-        <v>499</v>
+        <v>398</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>32</v>
@@ -972,13 +1017,13 @@
     </row>
     <row r="34" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1">
-        <v>458</v>
+        <v>196</v>
       </c>
       <c r="C34" s="1">
-        <v>105</v>
+        <v>776</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>33</v>
@@ -986,13 +1031,13 @@
     </row>
     <row r="35" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B35" s="1">
-        <v>481</v>
+        <v>620</v>
       </c>
       <c r="C35" s="1">
-        <v>653</v>
+        <v>748</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>34</v>
@@ -1000,27 +1045,27 @@
     </row>
     <row r="36" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1">
-        <v>179</v>
+        <v>1240</v>
       </c>
       <c r="C36" s="1">
-        <v>654</v>
+        <v>633</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B37" s="1">
-        <v>641</v>
+        <v>113</v>
       </c>
       <c r="C37" s="1">
-        <v>329</v>
+        <v>1196</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>36</v>
@@ -1028,16 +1073,254 @@
     </row>
     <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B38" s="1">
-        <v>238</v>
+        <v>168</v>
       </c>
       <c r="C38" s="1">
-        <v>472</v>
+        <v>719</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="1">
+        <v>176</v>
+      </c>
+      <c r="C39" s="1">
+        <v>370</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="1">
+        <v>195</v>
+      </c>
+      <c r="C40" s="1">
+        <v>684</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="1">
+        <v>378</v>
+      </c>
+      <c r="C41" s="1">
+        <v>321</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="1">
+        <v>176</v>
+      </c>
+      <c r="C42" s="1">
+        <v>844</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="1">
+        <v>195</v>
+      </c>
+      <c r="C43" s="1">
+        <v>776</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="1">
+        <v>296</v>
+      </c>
+      <c r="C44" s="1">
+        <v>686</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="1">
+        <v>27</v>
+      </c>
+      <c r="C45" s="1">
+        <v>975</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="1">
+        <v>391</v>
+      </c>
+      <c r="C46" s="1">
+        <v>246</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="1">
+        <v>530</v>
+      </c>
+      <c r="C47" s="1">
+        <v>691</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="1">
+        <v>336</v>
+      </c>
+      <c r="C48" s="1">
+        <v>674</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="1">
+        <v>64</v>
+      </c>
+      <c r="C49" s="1">
+        <v>334</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="1">
+        <v>390</v>
+      </c>
+      <c r="C50" s="1">
+        <v>246</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="1">
+        <v>157</v>
+      </c>
+      <c r="C51" s="1">
+        <v>780</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="1">
+        <v>177</v>
+      </c>
+      <c r="C52" s="1">
+        <v>207</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="1">
+        <v>67</v>
+      </c>
+      <c r="C53" s="1">
+        <v>774</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="1">
+        <v>225</v>
+      </c>
+      <c r="C54" s="1">
+        <v>104</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1">
+        <v>642</v>
+      </c>
+      <c r="C55" s="1">
+        <v>329</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>